<commit_message>
added SN ratio in excel
</commit_message>
<xml_diff>
--- a/AIIoU summary.xlsx
+++ b/AIIoU summary.xlsx
@@ -1,27 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LocalAdmin\Documents\Zijue\Carbon-Fiber-Detection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a12/Desktop/Carbon-Fiber-Detection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A472E9-4A2B-4CDE-A9DC-5B91325689F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4822C61-A3A9-324F-BF70-A0D816850EA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10000" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="168">
   <si>
     <t>Pic_name</t>
   </si>
@@ -480,13 +492,58 @@
   </si>
   <si>
     <t>Nylon Feed rate</t>
+  </si>
+  <si>
+    <t>Lv1</t>
+  </si>
+  <si>
+    <t>Lv2</t>
+  </si>
+  <si>
+    <t>Lv3</t>
+  </si>
+  <si>
+    <t>Lv4</t>
+  </si>
+  <si>
+    <t>Arc Printing Speed</t>
+  </si>
+  <si>
+    <t>Arc Fibre Feed Rate</t>
+  </si>
+  <si>
+    <t>Arc Nylon Feed Rate</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Max-min</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Best setting</t>
+  </si>
+  <si>
+    <t>fiber feed rate is the most important factor, better to set highest at 1.1</t>
+  </si>
+  <si>
+    <t>nylon and printing temperature don't have too much influence on results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generally speaking, the slower the printing speed and the higher the fiber feed rate the more accurate the trajectory is </t>
+  </si>
+  <si>
+    <t>with radius increasing, the influence of factors increase compared with error, small radius's trajectory is more prone to noise</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -506,6 +563,19 @@
       <sz val="10.5"/>
       <color theme="1"/>
       <name val="DengXian"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -595,7 +665,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -615,6 +685,8 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -959,9 +1031,9 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -975,7 +1047,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -992,7 +1064,7 @@
         <v>0.79594138280371562</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1009,7 +1081,7 @@
         <v>0.8025762962044134</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1026,7 +1098,7 @@
         <v>0.76106489808827249</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1043,7 +1115,7 @@
         <v>0.81959865683071076</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1060,7 +1132,7 @@
         <v>0.7790387511979221</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1077,7 +1149,7 @@
         <v>0.78718689299080891</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1094,7 +1166,7 @@
         <v>0.69224491216561335</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1111,7 +1183,7 @@
         <v>0.72251656928665975</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1128,7 +1200,7 @@
         <v>0.76670039572122684</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1145,7 +1217,7 @@
         <v>0.70511931503727265</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1162,7 +1234,7 @@
         <v>0.71819534323307077</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1179,7 +1251,7 @@
         <v>0.69130186780285807</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1196,7 +1268,7 @@
         <v>0.80557659455344321</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1213,7 +1285,7 @@
         <v>0.71913691966794679</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1230,7 +1302,7 @@
         <v>0.69587635611294552</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1247,7 +1319,7 @@
         <v>0.84945381071402981</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1264,7 +1336,7 @@
         <v>0.70152333771591036</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1281,7 +1353,7 @@
         <v>0.65873915038223996</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1298,7 +1370,7 @@
         <v>0.65954474484157832</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1315,7 +1387,7 @@
         <v>0.57876453771189884</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1332,7 +1404,7 @@
         <v>0.67431864179254952</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1349,7 +1421,7 @@
         <v>0.62771014168956119</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1366,7 +1438,7 @@
         <v>0.63158128964156379</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1383,7 +1455,7 @@
         <v>0.63873624252687922</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1400,7 +1472,7 @@
         <v>0.6545000593805993</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1417,7 +1489,7 @@
         <v>0.70245106254983281</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1434,7 +1506,7 @@
         <v>0.75817782897499453</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1451,7 +1523,7 @@
         <v>0.65099168346668512</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1468,7 +1540,7 @@
         <v>0.72294556098345764</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1485,7 +1557,7 @@
         <v>0.70247608715565457</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1502,7 +1574,7 @@
         <v>0.77960679638967612</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1519,7 +1591,7 @@
         <v>0.65657259090824238</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1536,7 +1608,7 @@
         <v>0.68648509185048423</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1553,7 +1625,7 @@
         <v>0.58833968785463786</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1570,7 +1642,7 @@
         <v>0.62293271033571762</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1587,7 +1659,7 @@
         <v>0.64033360071139378</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1604,7 +1676,7 @@
         <v>0.72817947508669711</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1621,7 +1693,7 @@
         <v>0.75856189057062295</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1638,7 +1710,7 @@
         <v>0.80583910262744507</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1655,7 +1727,7 @@
         <v>0.76048833893289469</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1672,7 +1744,7 @@
         <v>0.7101090921720864</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1689,7 +1761,7 @@
         <v>0.69793651572128412</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1706,7 +1778,7 @@
         <v>0.8493938626055515</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1723,7 +1795,7 @@
         <v>0.67418032776230041</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1740,7 +1812,7 @@
         <v>0.69394139150079348</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1757,7 +1829,7 @@
         <v>0.75446720697657699</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1774,7 +1846,7 @@
         <v>0.66153901480815369</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1791,7 +1863,7 @@
         <v>0.66333210387261854</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1808,7 +1880,7 @@
         <v>0.75907656200257656</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1825,7 +1897,7 @@
         <v>0.73269860844195789</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1842,7 +1914,7 @@
         <v>0.73772405274251052</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1859,7 +1931,7 @@
         <v>0.76506505992142226</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1876,7 +1948,7 @@
         <v>0.68058822718879142</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -1893,7 +1965,7 @@
         <v>0.7365657415905269</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -1910,7 +1982,7 @@
         <v>0.76030903825076834</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -1927,7 +1999,7 @@
         <v>0.76599432089599029</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -1944,7 +2016,7 @@
         <v>0.73463779220197312</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -1961,7 +2033,7 @@
         <v>0.72242132516989577</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -1978,7 +2050,7 @@
         <v>0.65901741275223991</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -1995,7 +2067,7 @@
         <v>0.69173826737728716</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2012,7 +2084,7 @@
         <v>0.57371462356650138</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2029,7 +2101,7 @@
         <v>0.66987227403478689</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2046,7 +2118,7 @@
         <v>0.66186333938912489</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2063,7 +2135,7 @@
         <v>0.94666717007287671</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2080,7 +2152,7 @@
         <v>0.69727567919562261</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2097,7 +2169,7 @@
         <v>0.70620032841397395</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2114,7 +2186,7 @@
         <v>0.68317592085416012</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2131,7 +2203,7 @@
         <v>0.76212940902306714</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2148,7 +2220,7 @@
         <v>0.70132814273463073</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2165,7 +2237,7 @@
         <v>0.66403231612088054</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2182,7 +2254,7 @@
         <v>0.69292913992213945</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2199,7 +2271,7 @@
         <v>0.79614271419706628</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2216,7 +2288,7 @@
         <v>0.76789282247946367</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -2233,7 +2305,7 @@
         <v>0.82453407106709375</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -2250,7 +2322,7 @@
         <v>0.76624324613085226</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -2267,7 +2339,7 @@
         <v>0.80607046531606641</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -2284,7 +2356,7 @@
         <v>0.77134180052419699</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -2301,7 +2373,7 @@
         <v>0.82282246938561454</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -2318,7 +2390,7 @@
         <v>0.75835290327355909</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -2335,7 +2407,7 @@
         <v>0.76203843792625625</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2352,7 +2424,7 @@
         <v>0.6692761869724051</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2369,7 +2441,7 @@
         <v>0.69915913557980358</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -2386,7 +2458,7 @@
         <v>0.69884026994637827</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -2403,7 +2475,7 @@
         <v>0.71093633477899254</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -2420,7 +2492,7 @@
         <v>0.69297233355458432</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -2437,7 +2509,7 @@
         <v>0.67255777362464919</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -2454,7 +2526,7 @@
         <v>0.6628667464854785</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -2471,7 +2543,7 @@
         <v>0.64877894478576781</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -2488,7 +2560,7 @@
         <v>0.6565165344772772</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -2505,7 +2577,7 @@
         <v>0.68372727159960622</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -2522,7 +2594,7 @@
         <v>0.70399345784785683</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -2539,7 +2611,7 @@
         <v>0.70795957265013731</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -2556,7 +2628,7 @@
         <v>0.64989483197962217</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -2573,7 +2645,7 @@
         <v>0.77430002377012652</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -2590,7 +2662,7 @@
         <v>0.67364848987944614</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -2607,7 +2679,7 @@
         <v>0.65854518350688007</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -2624,7 +2696,7 @@
         <v>0.89908711646376627</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -2641,7 +2713,7 @@
         <v>0.8265266250079466</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -2658,7 +2730,7 @@
         <v>0.75197621762210898</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -2675,7 +2747,7 @@
         <v>0.81240067938044536</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -2692,7 +2764,7 @@
         <v>0.78015544236749401</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -2709,7 +2781,7 @@
         <v>0.7403882230558585</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -2726,7 +2798,7 @@
         <v>0.65470094245837718</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -2743,7 +2815,7 @@
         <v>0.72106744232356601</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -2760,7 +2832,7 @@
         <v>0.71620952408563654</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -2777,7 +2849,7 @@
         <v>0.63263321643772052</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -2794,7 +2866,7 @@
         <v>0.70568622200373199</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -2811,7 +2883,7 @@
         <v>0.70698766718733075</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -2828,7 +2900,7 @@
         <v>0.80346482492596483</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -2845,7 +2917,7 @@
         <v>0.72731841273477749</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -2862,7 +2934,7 @@
         <v>0.76084668082372398</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -2879,7 +2951,7 @@
         <v>0.69444859768980138</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -2896,7 +2968,7 @@
         <v>0.64291812315375385</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -2913,7 +2985,7 @@
         <v>0.68651252633158921</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -2930,7 +3002,7 @@
         <v>0.79940415827322742</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -2947,7 +3019,7 @@
         <v>0.79551662555759095</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -2964,7 +3036,7 @@
         <v>0.7343024117899033</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -2981,7 +3053,7 @@
         <v>0.78008402691350087</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -2998,7 +3070,7 @@
         <v>0.83355834720795685</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -3015,7 +3087,7 @@
         <v>0.80801489600532628</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -3032,7 +3104,7 @@
         <v>0.74173717757714974</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -3049,7 +3121,7 @@
         <v>0.67371370709745104</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -3066,7 +3138,7 @@
         <v>0.67154544398360483</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -3083,7 +3155,7 @@
         <v>0.73889179622923795</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -3100,7 +3172,7 @@
         <v>0.84664791983677978</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -3117,7 +3189,7 @@
         <v>0.65020760791229071</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -3134,7 +3206,7 @@
         <v>0.72103122728219415</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -3151,7 +3223,7 @@
         <v>0.68609181414253795</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -3168,7 +3240,7 @@
         <v>0.87088647795932661</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -3185,7 +3257,7 @@
         <v>0.72158617090337895</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -3202,7 +3274,7 @@
         <v>0.6804247947099068</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -3219,7 +3291,7 @@
         <v>0.68196219061992935</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -3236,7 +3308,7 @@
         <v>0.80883926800726258</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -3253,7 +3325,7 @@
         <v>0.71982919659176003</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -3270,7 +3342,7 @@
         <v>0.73633194787032952</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -3287,7 +3359,7 @@
         <v>0.71464531101999329</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -3304,7 +3376,7 @@
         <v>0.69463657037282844</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -3321,7 +3393,7 @@
         <v>0.6986164779156927</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -3338,7 +3410,7 @@
         <v>0.68143424084037296</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -3355,7 +3427,7 @@
         <v>0.73385518097958602</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -3372,7 +3444,7 @@
         <v>0.69336643451830571</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -3389,7 +3461,7 @@
         <v>0.58156649466543553</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -3406,7 +3478,7 @@
         <v>0.70899182615870548</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -3432,13 +3504,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{637E773F-A59B-4512-BDE5-EC0A21A85D74}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>148</v>
       </c>
@@ -3455,7 +3527,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -3472,7 +3544,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -3489,7 +3561,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -3506,7 +3578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -3523,7 +3595,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -3540,7 +3612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -3557,7 +3629,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -3574,7 +3646,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -3591,7 +3663,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -3608,7 +3680,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -3625,7 +3697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -3642,7 +3714,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -3659,7 +3731,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -3676,7 +3748,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -3693,7 +3765,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -3710,7 +3782,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -3730,4 +3802,611 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787548F2-B93C-CA4A-988D-AF189AE1710F}">
+  <dimension ref="A1:E37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" s="8">
+        <v>0.890548341173514</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0.98730590592894596</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0.27241858838497202</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0.82195529057692496</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" s="8">
+        <v>0.71138067945478101</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0.90972620273515803</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0.42584012801726001</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0.80284986514925605</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="8">
+        <v>0.80878412160368895</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0.729571151934443</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0.91508768051104605</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0.84648710323870002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" s="8">
+        <v>0.87562207435656403</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.665262980535822</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1.8363355255806699</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0.81285500018577805</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B6">
+        <f>MAX(B2:B5)-MIN(B2:B5)</f>
+        <v>0.179167661718733</v>
+      </c>
+      <c r="C6">
+        <f>MAX(C2:C5)-MIN(C2:C5)</f>
+        <v>0.32204292539312396</v>
+      </c>
+      <c r="D6">
+        <f>MAX(D2:D5)-MIN(D2:D5)</f>
+        <v>1.5639169371956978</v>
+      </c>
+      <c r="E6">
+        <f>MAX(E2:E5)-MIN(E2:E5)</f>
+        <v>4.3637238089443975E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7" s="8">
+        <v>3</v>
+      </c>
+      <c r="C7" s="8">
+        <v>2</v>
+      </c>
+      <c r="D7" s="8">
+        <v>1</v>
+      </c>
+      <c r="E7" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8" s="8">
+        <v>240</v>
+      </c>
+      <c r="C8" s="8">
+        <v>120</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10" s="8">
+        <v>0.37458165661107601</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.45216497287896401</v>
+      </c>
+      <c r="D10" s="8">
+        <v>5.8226500853988797E-2</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0.194002004234749</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0.116197649398056</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.271528035481512</v>
+      </c>
+      <c r="D11" s="8">
+        <v>9.2289117930815096E-2</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.37969110984525201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B12" s="8">
+        <v>0.29915710517473898</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.16338137915051901</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.218507670543622</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0.25065042445775898</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B13" s="8">
+        <v>0.39153256238292999</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.293759457422684</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.85338481839180402</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.35423538944121202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14">
+        <f>MAX(B10:B13)-MIN(B10:B13)</f>
+        <v>0.275334912984874</v>
+      </c>
+      <c r="C14">
+        <f>MAX(C10:C13)-MIN(C10:C13)</f>
+        <v>0.28878359372844498</v>
+      </c>
+      <c r="D14">
+        <f>MAX(D10:D13)-MIN(D10:D13)</f>
+        <v>0.79515831753781518</v>
+      </c>
+      <c r="E14">
+        <f>MAX(E10:E13)-MIN(E10:E13)</f>
+        <v>0.185689105610503</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B15" s="8">
+        <v>3</v>
+      </c>
+      <c r="C15" s="8">
+        <v>2</v>
+      </c>
+      <c r="D15" s="8">
+        <v>1</v>
+      </c>
+      <c r="E15" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>163</v>
+      </c>
+      <c r="B16" s="8">
+        <v>270</v>
+      </c>
+      <c r="C16" s="8">
+        <v>120</v>
+      </c>
+      <c r="D16" s="8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>153</v>
+      </c>
+      <c r="B18" s="8">
+        <v>1.0623989719023701</v>
+      </c>
+      <c r="C18" s="8">
+        <v>0.99223590533683803</v>
+      </c>
+      <c r="D18" s="8">
+        <v>0.341278980932334</v>
+      </c>
+      <c r="E18" s="8">
+        <v>0.96177805893017898</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>154</v>
+      </c>
+      <c r="B19" s="8">
+        <v>0.83842710900279205</v>
+      </c>
+      <c r="C19" s="8">
+        <v>1.0788857191741901</v>
+      </c>
+      <c r="D19" s="8">
+        <v>0.525986403683253</v>
+      </c>
+      <c r="E19" s="8">
+        <v>0.92957938133151896</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>155</v>
+      </c>
+      <c r="B20" s="8">
+        <v>0.90116299324368099</v>
+      </c>
+      <c r="C20" s="8">
+        <v>0.94687599210791495</v>
+      </c>
+      <c r="D20" s="8">
+        <v>1.10359406394213</v>
+      </c>
+      <c r="E20" s="8">
+        <v>0.98838156339882399</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>156</v>
+      </c>
+      <c r="B21" s="8">
+        <v>0.93789062568278203</v>
+      </c>
+      <c r="C21" s="8">
+        <v>0.72664478859799597</v>
+      </c>
+      <c r="D21" s="8">
+        <v>1.93920887715832</v>
+      </c>
+      <c r="E21" s="8">
+        <v>0.85817146336694605</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>161</v>
+      </c>
+      <c r="B22">
+        <f>MAX(B18:B21)-MIN(B18:B21)</f>
+        <v>0.22397186289957804</v>
+      </c>
+      <c r="C22">
+        <f>MAX(C18:C21)-MIN(C18:C21)</f>
+        <v>0.3522409305761941</v>
+      </c>
+      <c r="D22">
+        <f>MAX(D18:D21)-MIN(D18:D21)</f>
+        <v>1.597929896225986</v>
+      </c>
+      <c r="E22">
+        <f>MAX(E18:E21)-MIN(E18:E21)</f>
+        <v>0.13021010003187794</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B23" s="8">
+        <v>3</v>
+      </c>
+      <c r="C23" s="8">
+        <v>2</v>
+      </c>
+      <c r="D23" s="8">
+        <v>1</v>
+      </c>
+      <c r="E23" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>163</v>
+      </c>
+      <c r="B24" s="8">
+        <v>240</v>
+      </c>
+      <c r="C24" s="8">
+        <v>280</v>
+      </c>
+      <c r="D24" s="8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E24" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>153</v>
+      </c>
+      <c r="B26" s="8">
+        <v>1.2875234052525</v>
+      </c>
+      <c r="C26" s="8">
+        <v>1.59211120807738</v>
+      </c>
+      <c r="D26" s="8">
+        <v>0.42635952729655502</v>
+      </c>
+      <c r="E26" s="8">
+        <v>1.3963436223240799</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" s="8">
+        <v>1.2569463301085999</v>
+      </c>
+      <c r="C27" s="8">
+        <v>1.46536878943726</v>
+      </c>
+      <c r="D27" s="8">
+        <v>0.68087790556361605</v>
+      </c>
+      <c r="E27" s="8">
+        <v>1.1347794345600399</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>155</v>
+      </c>
+      <c r="B28" s="8">
+        <v>1.2830971281427299</v>
+      </c>
+      <c r="C28" s="8">
+        <v>1.14128029765947</v>
+      </c>
+      <c r="D28" s="8">
+        <v>1.5273696146726901</v>
+      </c>
+      <c r="E28" s="8">
+        <v>1.3766081177985201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>156</v>
+      </c>
+      <c r="B29" s="8">
+        <v>1.3509905516221601</v>
+      </c>
+      <c r="C29" s="8">
+        <v>1.00512700185226</v>
+      </c>
+      <c r="D29" s="8">
+        <v>2.9747220474691001</v>
+      </c>
+      <c r="E29" s="8">
+        <v>1.2752492560533599</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>161</v>
+      </c>
+      <c r="B30">
+        <f>MAX(B26:B29)-MIN(B26:B29)</f>
+        <v>9.4044221513560178E-2</v>
+      </c>
+      <c r="C30">
+        <f>MAX(C26:C29)-MIN(C26:C29)</f>
+        <v>0.58698420622512004</v>
+      </c>
+      <c r="D30">
+        <f>MAX(D26:D29)-MIN(D26:D29)</f>
+        <v>2.5483625201725451</v>
+      </c>
+      <c r="E30">
+        <f>MAX(E26:E29)-MIN(E26:E29)</f>
+        <v>0.26156418776404</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>162</v>
+      </c>
+      <c r="B31" s="8">
+        <v>4</v>
+      </c>
+      <c r="C31" s="8">
+        <v>2</v>
+      </c>
+      <c r="D31" s="8">
+        <v>1</v>
+      </c>
+      <c r="E31" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>163</v>
+      </c>
+      <c r="B32" s="8">
+        <v>270</v>
+      </c>
+      <c r="C32" s="8">
+        <v>120</v>
+      </c>
+      <c r="D32" s="8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E32" s="8">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:E5">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10:E13">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:E21">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26:E29">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finished SN ratio for ANOVA
</commit_message>
<xml_diff>
--- a/AIIoU summary.xlsx
+++ b/AIIoU summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a12/Desktop/Carbon-Fiber-Detection/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\61452\Desktop\Carbon-Fiber-Detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4822C61-A3A9-324F-BF70-A0D816850EA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B78FAEE-ED73-4689-BDA1-2B2F6B902F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10000" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5820" yWindow="0" windowWidth="23040" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -543,7 +543,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1027,13 +1027,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E145"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>0.79594138280371562</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>0.8025762962044134</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>0.76106489808827249</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>0.81959865683071076</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>0.7790387511979221</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>0.78718689299080891</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>0.69224491216561335</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>0.72251656928665975</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>0.76670039572122684</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>0.70511931503727265</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>0.71819534323307077</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>0.69130186780285807</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>0.80557659455344321</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>0.71913691966794679</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>0.69587635611294552</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>0.84945381071402981</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>0.70152333771591036</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>0.65873915038223996</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>0.65954474484157832</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>0.57876453771189884</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>0.67431864179254952</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1421,7 +1421,7 @@
         <v>0.62771014168956119</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>0.63158128964156379</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>0.63873624252687922</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>0.6545000593805993</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>0.70245106254983281</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>0.75817782897499453</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>0.65099168346668512</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>0.72294556098345764</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>0.70247608715565457</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>0.77960679638967612</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>0.65657259090824238</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>0.68648509185048423</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>0.58833968785463786</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>0.62293271033571762</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>0.64033360071139378</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>0.72817947508669711</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>0.75856189057062295</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>0.80583910262744507</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>0.76048833893289469</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>0.7101090921720864</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>0.69793651572128412</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>0.8493938626055515</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>0.67418032776230041</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>0.69394139150079348</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>0.75446720697657699</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>0.66153901480815369</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>0.66333210387261854</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>0.75907656200257656</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>0.73269860844195789</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>0.73772405274251052</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>0.76506505992142226</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>0.68058822718879142</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>0.7365657415905269</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>0.76030903825076834</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>0.76599432089599029</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>0.73463779220197312</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>0.72242132516989577</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2050,7 +2050,7 @@
         <v>0.65901741275223991</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2067,7 +2067,7 @@
         <v>0.69173826737728716</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>0.57371462356650138</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>0.66987227403478689</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2118,7 +2118,7 @@
         <v>0.66186333938912489</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>0.94666717007287671</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>0.69727567919562261</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>0.70620032841397395</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>0.68317592085416012</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>0.76212940902306714</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>0.70132814273463073</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>0.66403231612088054</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>0.69292913992213945</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>0.79614271419706628</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>0.76789282247946367</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>0.82453407106709375</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>0.76624324613085226</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>0.80607046531606641</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>0.77134180052419699</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>0.82282246938561454</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>0.75835290327355909</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>0.76203843792625625</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>0.6692761869724051</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>0.69915913557980358</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -2458,7 +2458,7 @@
         <v>0.69884026994637827</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>0.71093633477899254</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>0.69297233355458432</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>0.67255777362464919</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>0.6628667464854785</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>0.64877894478576781</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -2560,7 +2560,7 @@
         <v>0.6565165344772772</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>0.68372727159960622</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>0.70399345784785683</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>0.70795957265013731</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>0.64989483197962217</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>0.77430002377012652</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>0.67364848987944614</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>0.65854518350688007</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>0.89908711646376627</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>0.8265266250079466</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>0.75197621762210898</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -2747,7 +2747,7 @@
         <v>0.81240067938044536</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -2764,7 +2764,7 @@
         <v>0.78015544236749401</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>0.7403882230558585</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>0.65470094245837718</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>0.72106744232356601</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -2832,7 +2832,7 @@
         <v>0.71620952408563654</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>0.63263321643772052</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>0.70568622200373199</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -2883,7 +2883,7 @@
         <v>0.70698766718733075</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>0.80346482492596483</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>0.72731841273477749</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -2934,7 +2934,7 @@
         <v>0.76084668082372398</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>0.69444859768980138</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>0.64291812315375385</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>0.68651252633158921</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>0.79940415827322742</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>0.79551662555759095</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -3036,7 +3036,7 @@
         <v>0.7343024117899033</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>0.78008402691350087</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>0.83355834720795685</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>0.80801489600532628</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>0.74173717757714974</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>0.67371370709745104</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>0.67154544398360483</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -3155,7 +3155,7 @@
         <v>0.73889179622923795</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -3172,7 +3172,7 @@
         <v>0.84664791983677978</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -3189,7 +3189,7 @@
         <v>0.65020760791229071</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -3206,7 +3206,7 @@
         <v>0.72103122728219415</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:5">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>0.68609181414253795</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>0.87088647795932661</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:5">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -3257,7 +3257,7 @@
         <v>0.72158617090337895</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:5">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -3274,7 +3274,7 @@
         <v>0.6804247947099068</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:5">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>0.68196219061992935</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:5">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -3308,7 +3308,7 @@
         <v>0.80883926800726258</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:5">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -3325,7 +3325,7 @@
         <v>0.71982919659176003</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:5">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>0.73633194787032952</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:5">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>0.71464531101999329</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:5">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -3376,7 +3376,7 @@
         <v>0.69463657037282844</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:5">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -3393,7 +3393,7 @@
         <v>0.6986164779156927</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:5">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>0.68143424084037296</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:5">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -3427,7 +3427,7 @@
         <v>0.73385518097958602</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:5">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -3444,7 +3444,7 @@
         <v>0.69336643451830571</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:5">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -3461,7 +3461,7 @@
         <v>0.58156649466543553</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:5">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -3478,7 +3478,7 @@
         <v>0.70899182615870548</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:5">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -3504,13 +3504,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{637E773F-A59B-4512-BDE5-EC0A21A85D74}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="42" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>148</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15" thickBot="1">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15" thickBot="1">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -3561,7 +3561,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15" thickBot="1">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15" thickBot="1">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -3595,7 +3595,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15" thickBot="1">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -3612,7 +3612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15" thickBot="1">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15" thickBot="1">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15" thickBot="1">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15" thickBot="1">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15" thickBot="1">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -3697,7 +3697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15" thickBot="1">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -3714,7 +3714,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15" thickBot="1">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -3731,7 +3731,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15" thickBot="1">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15" thickBot="1">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15" thickBot="1">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -3782,7 +3782,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15" thickBot="1">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -3808,13 +3808,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{787548F2-B93C-CA4A-988D-AF189AE1710F}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15.6">
       <c r="A1" t="s">
         <v>160</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="18">
       <c r="A2" t="s">
         <v>153</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>0.82195529057692496</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="18">
       <c r="A3" t="s">
         <v>154</v>
       </c>
@@ -3865,7 +3865,7 @@
         <v>0.80284986514925605</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="18">
       <c r="A4" t="s">
         <v>155</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>0.84648710323870002</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="18">
       <c r="A5" t="s">
         <v>156</v>
       </c>
@@ -3899,7 +3899,7 @@
         <v>0.81285500018577805</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>161</v>
       </c>
@@ -3920,7 +3920,7 @@
         <v>4.3637238089443975E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="18">
       <c r="A7" t="s">
         <v>162</v>
       </c>
@@ -3937,7 +3937,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="18">
       <c r="A8" t="s">
         <v>163</v>
       </c>
@@ -3954,12 +3954,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="18">
       <c r="A10" t="s">
         <v>153</v>
       </c>
@@ -3976,7 +3976,7 @@
         <v>0.194002004234749</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="18">
       <c r="A11" t="s">
         <v>154</v>
       </c>
@@ -3993,7 +3993,7 @@
         <v>0.37969110984525201</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="18">
       <c r="A12" t="s">
         <v>155</v>
       </c>
@@ -4010,7 +4010,7 @@
         <v>0.25065042445775898</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="18">
       <c r="A13" t="s">
         <v>156</v>
       </c>
@@ -4027,7 +4027,7 @@
         <v>0.35423538944121202</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>161</v>
       </c>
@@ -4048,7 +4048,7 @@
         <v>0.185689105610503</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="18">
       <c r="A15" t="s">
         <v>162</v>
       </c>
@@ -4065,7 +4065,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="18">
       <c r="A16" t="s">
         <v>163</v>
       </c>
@@ -4082,12 +4082,12 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="18">
       <c r="A18" t="s">
         <v>153</v>
       </c>
@@ -4104,7 +4104,7 @@
         <v>0.96177805893017898</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="18">
       <c r="A19" t="s">
         <v>154</v>
       </c>
@@ -4121,7 +4121,7 @@
         <v>0.92957938133151896</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="18">
       <c r="A20" t="s">
         <v>155</v>
       </c>
@@ -4138,7 +4138,7 @@
         <v>0.98838156339882399</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="18">
       <c r="A21" t="s">
         <v>156</v>
       </c>
@@ -4155,7 +4155,7 @@
         <v>0.85817146336694605</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>161</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>0.13021010003187794</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="18">
       <c r="A23" t="s">
         <v>162</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="18">
       <c r="A24" t="s">
         <v>163</v>
       </c>
@@ -4210,12 +4210,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="18">
       <c r="A26" t="s">
         <v>153</v>
       </c>
@@ -4232,7 +4232,7 @@
         <v>1.3963436223240799</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="18">
       <c r="A27" t="s">
         <v>154</v>
       </c>
@@ -4249,7 +4249,7 @@
         <v>1.1347794345600399</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="18">
       <c r="A28" t="s">
         <v>155</v>
       </c>
@@ -4266,7 +4266,7 @@
         <v>1.3766081177985201</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="18">
       <c r="A29" t="s">
         <v>156</v>
       </c>
@@ -4283,7 +4283,7 @@
         <v>1.2752492560533599</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>161</v>
       </c>
@@ -4304,7 +4304,7 @@
         <v>0.26156418776404</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="18">
       <c r="A31" t="s">
         <v>162</v>
       </c>
@@ -4321,7 +4321,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="18">
       <c r="A32" t="s">
         <v>163</v>
       </c>
@@ -4338,22 +4338,22 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1">
       <c r="A34" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1">
       <c r="A35" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1">
       <c r="A36" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1">
       <c r="A37" t="s">
         <v>167</v>
       </c>

</xml_diff>